<commit_message>
add comment and modification on python functions
</commit_message>
<xml_diff>
--- a/static/temp_save_request/temp_output.xlsx
+++ b/static/temp_save_request/temp_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK101"/>
+  <dimension ref="A1:AJ101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -614,11 +614,6 @@
           <t xml:space="preserve">Établissement co-accrédité </t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
-        <is>
-          <t>Id</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -801,9 +796,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK2" t="n">
-        <v>155</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -986,9 +978,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK3" t="n">
-        <v>156</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1171,9 +1160,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK4" t="n">
-        <v>157</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1356,9 +1342,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK5" t="n">
-        <v>158</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1541,9 +1524,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK6" t="n">
-        <v>159</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1726,9 +1706,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK7" t="n">
-        <v>160</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1911,9 +1888,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK8" t="n">
-        <v>161</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -2096,9 +2070,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK9" t="n">
-        <v>162</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2281,9 +2252,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK10" t="n">
-        <v>163</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2466,9 +2434,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK11" t="n">
-        <v>164</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2651,9 +2616,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK12" t="n">
-        <v>165</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2836,9 +2798,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK13" t="n">
-        <v>166</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -3021,9 +2980,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK14" t="n">
-        <v>167</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -3206,9 +3162,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK15" t="n">
-        <v>168</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -3391,9 +3344,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK16" t="n">
-        <v>169</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -3576,9 +3526,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK17" t="n">
-        <v>170</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -3761,9 +3708,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK18" t="n">
-        <v>171</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -3946,9 +3890,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK19" t="n">
-        <v>172</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -4131,9 +4072,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK20" t="n">
-        <v>173</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -4316,9 +4254,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK21" t="n">
-        <v>174</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -4501,9 +4436,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK22" t="n">
-        <v>175</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -4687,9 +4619,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK23" t="n">
-        <v>176</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -4872,9 +4801,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK24" t="n">
-        <v>177</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -5057,9 +4983,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK25" t="n">
-        <v>178</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -5242,9 +5165,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK26" t="n">
-        <v>179</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -5427,9 +5347,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK27" t="n">
-        <v>180</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -5612,9 +5529,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK28" t="n">
-        <v>181</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -5797,9 +5711,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK29" t="n">
-        <v>182</v>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -5982,9 +5893,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK30" t="n">
-        <v>183</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -6167,9 +6075,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK31" t="n">
-        <v>184</v>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -6352,9 +6257,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK32" t="n">
-        <v>185</v>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -6537,9 +6439,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK33" t="n">
-        <v>186</v>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -6722,9 +6621,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK34" t="n">
-        <v>187</v>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -6907,9 +6803,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK35" t="n">
-        <v>188</v>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -7092,9 +6985,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK36" t="n">
-        <v>189</v>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -7277,9 +7167,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK37" t="n">
-        <v>190</v>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -7462,9 +7349,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK38" t="n">
-        <v>191</v>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -7647,9 +7531,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK39" t="n">
-        <v>192</v>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -7832,9 +7713,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK40" t="n">
-        <v>193</v>
-      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -8017,9 +7895,6 @@
           <t xml:space="preserve"> Institut national des sciences appliquées Rouen Normandie (Saint-Etienne-du-Rouvray ; 1985-....)</t>
         </is>
       </c>
-      <c r="AK41" t="n">
-        <v>194</v>
-      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -8203,9 +8078,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK42" t="n">
-        <v>195</v>
-      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -8388,9 +8260,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK43" t="n">
-        <v>196</v>
-      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -8573,9 +8442,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK44" t="n">
-        <v>197</v>
-      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -8758,9 +8624,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK45" t="n">
-        <v>198</v>
-      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -8943,9 +8806,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK46" t="n">
-        <v>199</v>
-      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -9128,9 +8988,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK47" t="n">
-        <v>200</v>
-      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -9313,9 +9170,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK48" t="n">
-        <v>201</v>
-      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -9498,9 +9352,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK49" t="n">
-        <v>202</v>
-      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -9683,9 +9534,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK50" t="n">
-        <v>203</v>
-      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -9868,9 +9716,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK51" t="n">
-        <v>204</v>
-      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -10053,9 +9898,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK52" t="n">
-        <v>205</v>
-      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -10238,9 +10080,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK53" t="n">
-        <v>206</v>
-      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -10423,9 +10262,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK54" t="n">
-        <v>207</v>
-      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -10608,9 +10444,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK55" t="n">
-        <v>208</v>
-      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -10789,9 +10622,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK56" t="n">
-        <v>209</v>
-      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -10974,9 +10804,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK57" t="n">
-        <v>210</v>
-      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -11159,9 +10986,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK58" t="n">
-        <v>211</v>
-      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -11344,9 +11168,6 @@
           <t xml:space="preserve"> Université de Rouen Normandie (1966-....)</t>
         </is>
       </c>
-      <c r="AK59" t="n">
-        <v>212</v>
-      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -11529,9 +11350,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK60" t="n">
-        <v>213</v>
-      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -11714,9 +11532,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK61" t="n">
-        <v>214</v>
-      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -11899,9 +11714,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK62" t="n">
-        <v>215</v>
-      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -12084,9 +11896,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK63" t="n">
-        <v>216</v>
-      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -12269,9 +12078,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK64" t="n">
-        <v>217</v>
-      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -12454,9 +12260,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK65" t="n">
-        <v>218</v>
-      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -12639,9 +12442,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK66" t="n">
-        <v>219</v>
-      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -12824,9 +12624,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK67" t="n">
-        <v>220</v>
-      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -13009,9 +12806,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK68" t="n">
-        <v>221</v>
-      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -13194,9 +12988,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK69" t="n">
-        <v>222</v>
-      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -13379,9 +13170,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK70" t="n">
-        <v>223</v>
-      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -13564,9 +13352,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK71" t="n">
-        <v>224</v>
-      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -13749,9 +13534,6 @@
           <t xml:space="preserve"> Université de Rouen Normandie (1966-....)</t>
         </is>
       </c>
-      <c r="AK72" t="n">
-        <v>225</v>
-      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -13934,9 +13716,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK73" t="n">
-        <v>226</v>
-      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -14119,9 +13898,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK74" t="n">
-        <v>227</v>
-      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -14304,9 +14080,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK75" t="n">
-        <v>228</v>
-      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -14489,9 +14262,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK76" t="n">
-        <v>229</v>
-      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -14674,9 +14444,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK77" t="n">
-        <v>230</v>
-      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -14859,9 +14626,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK78" t="n">
-        <v>231</v>
-      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -15044,9 +14808,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK79" t="n">
-        <v>232</v>
-      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -15229,9 +14990,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK80" t="n">
-        <v>233</v>
-      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -15414,9 +15172,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK81" t="n">
-        <v>234</v>
-      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -15599,9 +15354,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK82" t="n">
-        <v>235</v>
-      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -15784,9 +15536,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK83" t="n">
-        <v>236</v>
-      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -15969,9 +15718,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK84" t="n">
-        <v>237</v>
-      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -16154,9 +15900,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK85" t="n">
-        <v>238</v>
-      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -16339,9 +16082,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK86" t="n">
-        <v>239</v>
-      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -16524,9 +16264,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK87" t="n">
-        <v>240</v>
-      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -16709,9 +16446,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK88" t="n">
-        <v>241</v>
-      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -16894,9 +16628,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK89" t="n">
-        <v>242</v>
-      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -17079,9 +16810,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK90" t="n">
-        <v>243</v>
-      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -17264,9 +16992,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK91" t="n">
-        <v>244</v>
-      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -17449,9 +17174,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK92" t="n">
-        <v>245</v>
-      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -17634,9 +17356,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK93" t="n">
-        <v>246</v>
-      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -17819,9 +17538,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK94" t="n">
-        <v>247</v>
-      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -18005,9 +17721,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK95" t="n">
-        <v>248</v>
-      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -18190,9 +17903,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK96" t="n">
-        <v>249</v>
-      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -18375,9 +18085,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK97" t="n">
-        <v>250</v>
-      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -18560,9 +18267,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK98" t="n">
-        <v>251</v>
-      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -18745,9 +18449,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK99" t="n">
-        <v>252</v>
-      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -18930,9 +18631,6 @@
           <t>Missing value</t>
         </is>
       </c>
-      <c r="AK100" t="n">
-        <v>253</v>
-      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -19114,9 +18812,6 @@
         <is>
           <t>Missing value</t>
         </is>
-      </c>
-      <c r="AK101" t="n">
-        <v>254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>